<commit_message>
20190904 1. Login and Logout改為post 2. reLoadSession小調整 3. restful/crud 底下改為需要有權限才能使用 4. excel調整 5. 小bug調整
</commit_message>
<xml_diff>
--- a/templates/(舊報機單X2)轉出關貿格式範例.xlsx
+++ b/templates/(舊報機單X2)轉出關貿格式範例.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Case\東風\原始碼\20170116_Module\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F58277-2954-4627-9938-8A3C04D9A28A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAEA663-89D4-4E43-BE58-7648A8864B36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="NGIUOW" sheetId="5" state="veryHidden" r:id="rId1"/>
-    <sheet name="報機明細" sheetId="1" r:id="rId2"/>
+    <sheet name="報機明細" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">報機明細!$A$4:$Q$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">報機明細!$A$4:$Q$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -203,26 +202,6 @@
   </si>
   <si>
     <t>${table:data.IL_NEWUNIT}</t>
-    <phoneticPr fontId="31" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>${table:data.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-      </rPr>
-      <t>IL_WEIGHT_NEW</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-      </rPr>
-      <t>}</t>
-    </r>
     <phoneticPr fontId="31" type="noConversion"/>
   </si>
   <si>
@@ -306,6 +285,10 @@
   <si>
     <t>${table:data.IL_G1_X2}</t>
     <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>${table:data.IL_WEIGHT_NEW_X2}</t>
+    <phoneticPr fontId="31" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1699,23 +1682,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
-  <sheetData/>
-  <phoneticPr fontId="23" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
@@ -1888,12 +1854,12 @@
         <v>19</v>
       </c>
       <c r="R4" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>34</v>
@@ -1911,7 +1877,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H5" s="30" t="s">
         <v>27</v>
@@ -1920,19 +1886,19 @@
         <v>35</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K5" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L5" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="N5" s="31" t="s">
         <v>38</v>
-      </c>
-      <c r="N5" s="31" t="s">
-        <v>39</v>
       </c>
       <c r="O5" s="30" t="s">
         <v>28</v>
@@ -1944,7 +1910,7 @@
         <v>31</v>
       </c>
       <c r="R5" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>